<commit_message>
CP Cam + Zcar
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang4/2.XuLyBH/XLBH2304_NhatQuang.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang4/2.XuLyBH/XLBH2304_NhatQuang.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
   <si>
     <t>STT</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Le4.1.04.BOO01.221222</t>
+  </si>
+  <si>
+    <t>TG102LE-4G(GD)</t>
   </si>
 </sst>
 </file>
@@ -646,6 +649,30 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -661,32 +688,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1030,41 +1033,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
+      <c r="A1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
       <c r="W1" s="36"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="79"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="4"/>
       <c r="H2" s="17"/>
       <c r="I2" s="40"/>
@@ -1097,57 +1100,57 @@
       <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="75"/>
-      <c r="L4" s="72" t="s">
+      <c r="K4" s="67"/>
+      <c r="L4" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="72" t="s">
+      <c r="M4" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="72" t="s">
+      <c r="N4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="72" t="s">
+      <c r="O4" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="70" t="s">
+      <c r="P4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="72" t="s">
+      <c r="Q4" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="R4" s="72" t="s">
+      <c r="R4" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="74" t="s">
+      <c r="S4" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="75" t="s">
+      <c r="U4" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="75" t="s">
+      <c r="V4" s="67" t="s">
         <v>52</v>
       </c>
       <c r="W4" s="37"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
@@ -1178,16 +1181,16 @@
       <c r="K5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="74"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="80"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
       <c r="W5" s="37"/>
     </row>
     <row r="6" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1221,7 +1224,7 @@
       <c r="R6" s="63"/>
       <c r="S6" s="64"/>
       <c r="T6" s="12"/>
-      <c r="U6" s="67" t="s">
+      <c r="U6" s="75" t="s">
         <v>17</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1252,7 +1255,7 @@
       <c r="R7" s="63"/>
       <c r="S7" s="64"/>
       <c r="T7" s="12"/>
-      <c r="U7" s="68"/>
+      <c r="U7" s="76"/>
       <c r="V7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1281,7 +1284,7 @@
       <c r="R8" s="63"/>
       <c r="S8" s="64"/>
       <c r="T8" s="12"/>
-      <c r="U8" s="68"/>
+      <c r="U8" s="76"/>
       <c r="V8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1310,7 +1313,7 @@
       <c r="R9" s="63"/>
       <c r="S9" s="64"/>
       <c r="T9" s="12"/>
-      <c r="U9" s="68"/>
+      <c r="U9" s="76"/>
       <c r="V9" s="3" t="s">
         <v>50</v>
       </c>
@@ -1339,7 +1342,7 @@
       <c r="R10" s="63"/>
       <c r="S10" s="64"/>
       <c r="T10" s="12"/>
-      <c r="U10" s="68"/>
+      <c r="U10" s="76"/>
       <c r="V10" s="3" t="s">
         <v>30</v>
       </c>
@@ -1368,7 +1371,7 @@
       <c r="R11" s="53"/>
       <c r="S11" s="55"/>
       <c r="T11" s="12"/>
-      <c r="U11" s="68"/>
+      <c r="U11" s="76"/>
       <c r="V11" s="3" t="s">
         <v>29</v>
       </c>
@@ -1397,7 +1400,7 @@
       <c r="R12" s="53"/>
       <c r="S12" s="3"/>
       <c r="T12" s="12"/>
-      <c r="U12" s="67" t="s">
+      <c r="U12" s="75" t="s">
         <v>18</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1428,7 +1431,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="12"/>
-      <c r="U13" s="68"/>
+      <c r="U13" s="76"/>
       <c r="V13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1457,7 +1460,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="12"/>
-      <c r="U14" s="68"/>
+      <c r="U14" s="76"/>
       <c r="V14" s="3" t="s">
         <v>35</v>
       </c>
@@ -1486,7 +1489,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="12"/>
-      <c r="U15" s="68"/>
+      <c r="U15" s="76"/>
       <c r="V15" s="3" t="s">
         <v>23</v>
       </c>
@@ -1515,7 +1518,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="12"/>
-      <c r="U16" s="69"/>
+      <c r="U16" s="77"/>
       <c r="V16" s="3" t="s">
         <v>24</v>
       </c>
@@ -3216,6 +3219,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3227,13 +3237,6 @@
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="L4:L5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3245,7 +3248,7 @@
   <dimension ref="A1:X57"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3277,41 +3280,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
+      <c r="A1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
       <c r="W1" s="36"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="79"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="4"/>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -3344,57 +3347,57 @@
       <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="75"/>
-      <c r="L4" s="72" t="s">
+      <c r="K4" s="67"/>
+      <c r="L4" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="72" t="s">
+      <c r="M4" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="72" t="s">
+      <c r="N4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="75" t="s">
+      <c r="O4" s="67" t="s">
         <v>6</v>
       </c>
       <c r="P4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="75" t="s">
+      <c r="Q4" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="R4" s="75" t="s">
+      <c r="R4" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="74" t="s">
+      <c r="S4" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="75" t="s">
+      <c r="U4" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="75" t="s">
+      <c r="V4" s="67" t="s">
         <v>52</v>
       </c>
       <c r="W4" s="37"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
@@ -3425,16 +3428,16 @@
       <c r="K5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="75"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="67"/>
       <c r="P5" s="81"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75"/>
-      <c r="S5" s="74"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="80"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
       <c r="W5" s="37"/>
     </row>
     <row r="6" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3448,7 +3451,7 @@
         <v>45034</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="E6" s="65">
         <v>862205051189191</v>
@@ -3488,7 +3491,7 @@
       </c>
       <c r="S6" s="64"/>
       <c r="T6" s="12"/>
-      <c r="U6" s="67" t="s">
+      <c r="U6" s="75" t="s">
         <v>17</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3519,7 +3522,7 @@
       <c r="R7" s="31"/>
       <c r="S7" s="3"/>
       <c r="T7" s="12"/>
-      <c r="U7" s="68"/>
+      <c r="U7" s="76"/>
       <c r="V7" s="3" t="s">
         <v>34</v>
       </c>
@@ -3548,7 +3551,7 @@
       <c r="R8" s="31"/>
       <c r="S8" s="3"/>
       <c r="T8" s="12"/>
-      <c r="U8" s="68"/>
+      <c r="U8" s="76"/>
       <c r="V8" s="3" t="s">
         <v>20</v>
       </c>
@@ -3577,7 +3580,7 @@
       <c r="R9" s="31"/>
       <c r="S9" s="3"/>
       <c r="T9" s="12"/>
-      <c r="U9" s="68"/>
+      <c r="U9" s="76"/>
       <c r="V9" s="3" t="s">
         <v>50</v>
       </c>
@@ -3606,7 +3609,7 @@
       <c r="R10" s="31"/>
       <c r="S10" s="3"/>
       <c r="T10" s="12"/>
-      <c r="U10" s="68"/>
+      <c r="U10" s="76"/>
       <c r="V10" s="3" t="s">
         <v>30</v>
       </c>
@@ -3635,7 +3638,7 @@
       <c r="R11" s="31"/>
       <c r="S11" s="3"/>
       <c r="T11" s="12"/>
-      <c r="U11" s="68"/>
+      <c r="U11" s="76"/>
       <c r="V11" s="3" t="s">
         <v>29</v>
       </c>
@@ -3664,7 +3667,7 @@
       <c r="R12" s="31"/>
       <c r="S12" s="3"/>
       <c r="T12" s="12"/>
-      <c r="U12" s="67" t="s">
+      <c r="U12" s="75" t="s">
         <v>18</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -3695,7 +3698,7 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="12"/>
-      <c r="U13" s="68"/>
+      <c r="U13" s="76"/>
       <c r="V13" s="3" t="s">
         <v>36</v>
       </c>
@@ -3724,7 +3727,7 @@
       <c r="R14" s="31"/>
       <c r="S14" s="3"/>
       <c r="T14" s="12"/>
-      <c r="U14" s="68"/>
+      <c r="U14" s="76"/>
       <c r="V14" s="3" t="s">
         <v>35</v>
       </c>
@@ -3753,7 +3756,7 @@
       <c r="R15" s="31"/>
       <c r="S15" s="3"/>
       <c r="T15" s="12"/>
-      <c r="U15" s="68"/>
+      <c r="U15" s="76"/>
       <c r="V15" s="3" t="s">
         <v>23</v>
       </c>
@@ -3782,7 +3785,7 @@
       <c r="R16" s="31"/>
       <c r="S16" s="3"/>
       <c r="T16" s="12"/>
-      <c r="U16" s="69"/>
+      <c r="U16" s="77"/>
       <c r="V16" s="3" t="s">
         <v>24</v>
       </c>
@@ -5013,13 +5016,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -5031,6 +5027,13 @@
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="L4:L5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>